<commit_message>
sửa lại import export kpi item
</commit_message>
<xml_diff>
--- a/DMS/Templates/Kpi_Item_Export.xlsx
+++ b/DMS/Templates/Kpi_Item_Export.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73A1A0B-8549-49B8-87D6-BDFDCA2B69F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102E61B1-F5D9-4E7D-A859-32BD45085FA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="KPI nhân viên" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'KPI nhân viên'!$A$4:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'KPI nhân viên'!$A$4:$G$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>Năm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Mã nhân viên</t>
   </si>
@@ -45,18 +42,9 @@
     <t>Mã sản phẩm</t>
   </si>
   <si>
-    <t>Kỳ</t>
-  </si>
-  <si>
     <t>Tên sản phẩm</t>
   </si>
   <si>
-    <t>{{KpiPeriod}}</t>
-  </si>
-  <si>
-    <t>{{KpiYear}}</t>
-  </si>
-  <si>
     <t>{{KpiItems.Username}} - {{KpiItems.DisplayName}}</t>
   </si>
   <si>
@@ -72,52 +60,58 @@
     <t>{{KpiItems.Contents.ItemName}}</t>
   </si>
   <si>
-    <t>Sản lượng theo đơn gián tiếp</t>
-  </si>
-  <si>
-    <t>Doanh thu theo đơn gián tiếp</t>
-  </si>
-  <si>
-    <t>Số đơn hàng theo đơn gián tiếp</t>
-  </si>
-  <si>
-    <t>Số đại lý theo đơn gián tiếp</t>
-  </si>
-  <si>
-    <t>Sản lượng theo đơn trực tiếp</t>
-  </si>
-  <si>
-    <t>Doanh thu theo đơn trực tiếp</t>
-  </si>
-  <si>
-    <t>Số đơn hàng theo đơn trực tiếp</t>
-  </si>
-  <si>
-    <t>Số đại lý theo đơn trực tiếp</t>
-  </si>
-  <si>
-    <t>{{KpiItems.Contents.IndirectQuantity}}</t>
-  </si>
-  <si>
     <t>{{KpiItems.Contents.IndirectRevenue}}</t>
   </si>
   <si>
-    <t>{{KpiItems.Contents.IndirectCounter}}</t>
-  </si>
-  <si>
     <t>{{KpiItems.Contents.IndirectStoreCounter}}</t>
   </si>
   <si>
-    <t>{{KpiItems.Contents.DirectQuantity}}</t>
-  </si>
-  <si>
-    <t>{{KpiItems.Contents.DirectRevenue}}</t>
-  </si>
-  <si>
-    <t>{{KpiItems.Contents.DirectCounter}}</t>
-  </si>
-  <si>
-    <t>{{KpiItems.Contents.DirectStoreCounter}}</t>
+    <t>Loại KPI sản phẩm</t>
+  </si>
+  <si>
+    <t>{{KpiItems.KpiItemType.Name}}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kỳ: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">{{KpiPeriod}} - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Năm: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{{KpiYear}}</t>
+    </r>
+  </si>
+  <si>
+    <t>Doanh thu</t>
+  </si>
+  <si>
+    <t>Số đại lý hiện diện</t>
   </si>
 </sst>
 </file>
@@ -128,7 +122,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -136,7 +130,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -144,12 +138,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +162,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -231,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -265,6 +265,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,91 +555,80 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="6" width="31.42578125" customWidth="1"/>
-    <col min="7" max="10" width="30.42578125" customWidth="1"/>
-    <col min="11" max="12" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="7.25" customWidth="1"/>
+    <col min="3" max="4" width="10.375" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="6" max="6" width="11.875" customWidth="1"/>
+    <col min="7" max="8" width="31.375" customWidth="1"/>
+    <col min="9" max="11" width="30.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
-      <c r="J1" s="2"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>1</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="12"/>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -644,63 +639,49 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
+      <c r="K5" s="14"/>
     </row>
-    <row r="6" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="J6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="D1:I1"/>
+  <mergeCells count="9">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A5:N5"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
DMS: Fix KpiItem Export
</commit_message>
<xml_diff>
--- a/DMS/Templates/Kpi_Item_Export.xlsx
+++ b/DMS/Templates/Kpi_Item_Export.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102E61B1-F5D9-4E7D-A859-32BD45085FA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2DF54C-9C15-44F8-AF9A-425E0BBBAC8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>Loại KPI sản phẩm</t>
   </si>
   <si>
-    <t>{{KpiItems.KpiItemType.Name}}</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Kỳ: </t>
     </r>
@@ -79,7 +76,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -90,7 +87,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -100,7 +97,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>Số đại lý hiện diện</t>
+  </si>
+  <si>
+    <t>{{KpiItems.KpiItemTypeName}}</t>
   </si>
 </sst>
 </file>
@@ -122,7 +122,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -130,7 +130,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -138,7 +138,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -245,29 +245,29 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -558,37 +558,37 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E6" sqref="E6:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="7.25" customWidth="1"/>
-    <col min="3" max="4" width="10.375" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="6" max="6" width="11.875" customWidth="1"/>
-    <col min="7" max="8" width="31.375" customWidth="1"/>
-    <col min="9" max="11" width="30.375" customWidth="1"/>
+    <col min="1" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="8" width="31.42578125" customWidth="1"/>
+    <col min="9" max="11" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -620,13 +620,13 @@
         <v>4</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -639,9 +639,9 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
+      <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -651,7 +651,7 @@
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="3" t="s">
@@ -667,12 +667,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C4:D4"/>
@@ -680,8 +682,6 @@
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>